<commit_message>
Changed outdated tests for Production. Added a printing of the stmtID if there is an error. Added test for offset of rows and columns
</commit_message>
<xml_diff>
--- a/core/exporter/production/testing/expected/01_TestProductionWithoutParsingError_CODED.xlsx
+++ b/core/exporter/production/testing/expected/01_TestProductionWithoutParsingError_CODED.xlsx
@@ -91,10 +91,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,8 +122,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,7 +408,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showGridLines="false" tabSelected="true" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -662,7 +668,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[OK]</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -864,7 +870,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[OK]</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -1066,7 +1072,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>[OK]</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -1268,7 +1274,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>[OK]</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -1470,7 +1476,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>[OK]</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1672,7 +1678,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>[OK]</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">

</xml_diff>